<commit_message>
Adding Firm Birth Rate Data
</commit_message>
<xml_diff>
--- a/New Business Boom/Remote_Work_Data.xlsx
+++ b/New Business Boom/Remote_Work_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\Documents\GitHub\Apricitas\New Business Boom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA562B33-7168-488C-A66F-5DCA08A10CEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AA47A11-6836-41CC-809F-9FFFF1A46CDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{F666AC94-0BCE-4025-99C1-3F89211CA064}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{F666AC94-0BCE-4025-99C1-3F89211CA064}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1270,15 +1270,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7605DD38-5099-4C45-AF45-2CE83B450FBA}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>7</v>
       </c>
@@ -1295,7 +1295,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1317,7 +1317,7 @@
         <v>9.0133191847488012E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1338,8 +1338,16 @@
         <f t="shared" si="0"/>
         <v>0.1352230971128609</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <f>(B3+B2)/($D2+$D3)</f>
+        <v>0.17672330149421075</v>
+      </c>
+      <c r="I3">
+        <f>(C3+C2)/($D2+$D3)</f>
+        <v>0.10865370102848272</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1361,7 +1369,7 @@
         <v>0.10650315261085151</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1392,7 +1400,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E9CCD08-46D8-4C6C-9DD7-985D3CAE9228}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>

</xml_diff>